<commit_message>
Form UI and validations
</commit_message>
<xml_diff>
--- a/src/app/data/EJEMPLO.xlsx
+++ b/src/app/data/EJEMPLO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOD_PAGE\fod-pagina\src\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C36BCE-4900-4307-A5EF-1488654166E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4664C0AA-435C-4C77-8D9A-CB005300C204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73DE6B6D-A6E2-4231-B8D2-CE5820BC0412}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Edad</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A3FF1E-C176-48CE-B778-8BDAF60C4B6D}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +481,7 @@
     <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,25 +489,28 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -512,25 +518,28 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>34</v>
+      </c>
+      <c r="D2">
         <v>2.5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>70</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>85</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>12.4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>199.9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -538,25 +547,28 @@
         <v>2</v>
       </c>
       <c r="C3">
+        <v>53</v>
+      </c>
+      <c r="D3">
         <v>1.8</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>65</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>35</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>78</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>10.9</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>190.7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -564,25 +576,28 @@
         <v>3</v>
       </c>
       <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>80</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>28</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>82</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>11.3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>203.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -590,25 +605,28 @@
         <v>4</v>
       </c>
       <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
         <v>1.9</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>60</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>32</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>76</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>13</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>182.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -616,25 +634,28 @@
         <v>5</v>
       </c>
       <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>75</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>29</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>80</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>12.7</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>198.7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -642,25 +663,28 @@
         <v>6</v>
       </c>
       <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>72</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>33</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>84</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>11.6</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>202.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -668,25 +692,28 @@
         <v>7</v>
       </c>
       <c r="C8">
+        <v>42</v>
+      </c>
+      <c r="D8">
         <v>2.1</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>68</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>31</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>79</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>12.9</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -694,25 +721,28 @@
         <v>8</v>
       </c>
       <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>67</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>34</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>77</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>12.1</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>192.1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -720,25 +750,28 @@
         <v>9</v>
       </c>
       <c r="C10">
+        <v>32</v>
+      </c>
+      <c r="D10">
         <v>1.8</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>69</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>30</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>75</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>13.5</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>189.3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -746,21 +779,24 @@
         <v>10</v>
       </c>
       <c r="C11">
+        <v>47</v>
+      </c>
+      <c r="D11">
         <v>2.4</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>74</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>32</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>81</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>11.9</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>201.3</v>
       </c>
     </row>

</xml_diff>